<commit_message>
Added schema validator and new test cases
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\IdeaProjects\RestAssured_PetShop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F90736-4271-4195-809D-65AF897EB077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CA0000-ADAE-4297-89AE-6106993960B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -387,7 +387,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -437,8 +437,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -725,7 +724,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,7 +733,7 @@
     <col min="2" max="2" width="25.42578125" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="48.42578125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="48.42578125" customWidth="1"/>
     <col min="6" max="6" width="23.7109375" customWidth="1"/>
     <col min="7" max="7" width="28.85546875" customWidth="1"/>
     <col min="8" max="8" width="28.28515625" customWidth="1"/>
@@ -792,30 +791,30 @@
         <v>15</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="10"/>
+        <v>28</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="H2" s="10"/>
-      <c r="I2" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="I2" s="7"/>
       <c r="J2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="14">
+      <c r="K2" s="7"/>
+      <c r="L2" s="6">
         <v>200</v>
       </c>
-      <c r="M2" s="11"/>
+      <c r="M2" s="7"/>
     </row>
     <row r="3" spans="1:13" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
@@ -823,12 +822,12 @@
         <v>15</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -842,11 +841,11 @@
       <c r="J3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="13">
+      <c r="K3" s="12"/>
+      <c r="L3" s="14">
         <v>200</v>
       </c>
-      <c r="M3" s="7"/>
+      <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:13" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
@@ -854,27 +853,27 @@
         <v>15</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G4" s="10"/>
-      <c r="H4" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="7"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="J4" s="7" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="K4" s="7"/>
-      <c r="L4" s="6">
+      <c r="L4" s="13">
         <v>200</v>
       </c>
       <c r="M4" s="7"/>
@@ -885,20 +884,20 @@
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7" t="s">
@@ -916,24 +915,24 @@
         <v>15</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="10"/>
+        <v>25</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10" t="s">
+        <v>27</v>
+      </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="6">
@@ -952,7 +951,7 @@
       <c r="D7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="9" t="s">
@@ -981,7 +980,7 @@
       <c r="D8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="9" t="s">
@@ -1004,7 +1003,7 @@
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="9"/>
@@ -1021,7 +1020,7 @@
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="9"/>
@@ -1038,7 +1037,7 @@
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="9"/>
@@ -1055,7 +1054,7 @@
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F12" s="9"/>
@@ -1072,7 +1071,7 @@
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F13" s="9"/>
@@ -1089,7 +1088,7 @@
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F14" s="9"/>
@@ -1106,7 +1105,7 @@
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="9"/>
@@ -1123,7 +1122,7 @@
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F16" s="9"/>
@@ -1140,7 +1139,7 @@
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F17" s="9"/>
@@ -1157,7 +1156,7 @@
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F18" s="9"/>
@@ -1174,7 +1173,7 @@
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F19" s="9"/>
@@ -1191,7 +1190,7 @@
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="9"/>
@@ -1208,7 +1207,7 @@
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F21" s="9"/>
@@ -1225,7 +1224,7 @@
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F22" s="9"/>
@@ -1242,7 +1241,7 @@
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F23" s="9"/>
@@ -1259,7 +1258,7 @@
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F24" s="9"/>
@@ -1276,7 +1275,7 @@
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F25" s="9"/>

</xml_diff>